<commit_message>
Framework is ready without listener
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ClientsDataExcel.xlsx
+++ b/src/test/resources/testdata/ClientsDataExcel.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PERSONAL_PROJECT_AUTO_TEST\AutomationFrameworkSelenium\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mywork\automation\Selenium\SeleniumFrameWork\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78044C1B-7A52-43FF-8F95-FDA5DBC034EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566ECBC3-F194-4D85-888C-EACC1C398494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="1836" windowWidth="18600" windowHeight="10224" activeTab="1" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A35AAC3-973C-4AA0-816A-DECEFD0ED1D8}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="3" r:id="rId1"/>
     <sheet name="Client" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -655,23 +655,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF288A0-DB40-4E38-9AAF-ADDED2880E84}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.21875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" style="10" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.28515625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.85546875" style="10" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="38" style="10" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5546875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.44140625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.33203125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="8.88671875" style="10" collapsed="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="4" max="4" width="18.5703125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.42578125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.28515625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="8.85546875" style="10" collapsed="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -691,7 +691,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>31</v>
       </c>
@@ -709,7 +709,7 @@
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>31</v>
       </c>
@@ -739,29 +739,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E2E380-41FF-438A-822D-1CBE2A443631}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.21875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.88671875" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="9" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="4.77734375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="24.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="4.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="8" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="18.21875" style="2" collapsed="1"/>
+    <col min="14" max="16384" width="18.28515625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
@@ -802,7 +802,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -840,7 +840,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -878,7 +878,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>

</xml_diff>